<commit_message>
New session stats generated
</commit_message>
<xml_diff>
--- a/Outputs/My Bankroll.xlsx
+++ b/Outputs/My Bankroll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\OneDrive\Documents\GitHub\Poker-Stats\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C6CC6C-5068-4B2E-B532-E84B577AACAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C976AE-405E-439D-AABD-CD649819706A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9632453-612A-44A0-BDF1-31A9056B2690}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -261,9 +261,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Bankroll</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -348,10 +345,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>44294</c:v>
                 </c:pt>
@@ -384,16 +381,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>44331</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$12</c:f>
+              <c:f>Sheet1!$G$2:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>10.050000000000001</c:v>
                 </c:pt>
@@ -426,6 +426,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>192.53000000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>273.97000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -456,9 +459,6 @@
               <c15:ser>
                 <c:idx val="1"/>
                 <c:order val="1"/>
-                <c:tx>
-                  <c:v>Own Money Invested</c:v>
-                </c:tx>
                 <c:spPr>
                   <a:ln w="28575" cap="rnd">
                     <a:solidFill>
@@ -491,13 +491,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$2:$A$12</c15:sqref>
+                          <c15:sqref>Sheet1!$A$2:$A$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>d\-mmm</c:formatCode>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:pt idx="0">
                         <c:v>44294</c:v>
                       </c:pt>
@@ -530,6 +530,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>44331</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>44333</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -539,13 +542,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$H$2:$H$12</c15:sqref>
+                          <c15:sqref>Sheet1!$H$2:$H$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                       <c:pt idx="0">
                         <c:v>10.050000000000001</c:v>
                       </c:pt>
@@ -577,6 +580,9 @@
                         <c:v>10.050000000000001</c:v>
                       </c:pt>
                       <c:pt idx="10">
+                        <c:v>10.050000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
                         <c:v>10.050000000000001</c:v>
                       </c:pt>
                     </c:numCache>
@@ -1665,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF3161B-F657-4AAE-92D7-BE65727B2E9C}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1995,6 +2001,31 @@
         <v>14</v>
       </c>
     </row>
+    <row r="13" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>44333</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2">
+        <v>101.44</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13-D13</f>
+        <v>81.44</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" ref="G13" si="1">G12+F13</f>
+        <v>273.97000000000003</v>
+      </c>
+      <c r="H13" s="4">
+        <v>10.050000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>